<commit_message>
Implement get one, create and update model
</commit_message>
<xml_diff>
--- a/WebContent/WEB-INF/data/db.xlsx
+++ b/WebContent/WEB-INF/data/db.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -45,6 +45,60 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>new product</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>new prodct</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>My p</t>
+  </si>
+  <si>
+    <t>My pee</t>
   </si>
 </sst>
 </file>
@@ -89,7 +143,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,7 +171,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -128,13 +182,173 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>